<commit_message>
Hello i am adding something
</commit_message>
<xml_diff>
--- a/DataDrivenFramework/testdata/testdata.xlsx
+++ b/DataDrivenFramework/testdata/testdata.xlsx
@@ -14,22 +14,93 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="23">
   <si>
     <t>UserName</t>
   </si>
   <si>
     <t>Password</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Qualification</t>
+  </si>
+  <si>
+    <t>dbhatt</t>
+  </si>
+  <si>
+    <t>raj</t>
+  </si>
+  <si>
+    <t>mohita</t>
+  </si>
+  <si>
+    <t>Balram</t>
+  </si>
+  <si>
+    <t>Nellam</t>
+  </si>
+  <si>
+    <t>Sonu</t>
+  </si>
+  <si>
+    <t>Hema</t>
+  </si>
+  <si>
+    <t>Namita</t>
+  </si>
+  <si>
+    <t>Tesy@123</t>
+  </si>
+  <si>
+    <t>Test@123</t>
+  </si>
+  <si>
+    <t>damomca@gmail.com</t>
+  </si>
+  <si>
+    <t>user@user.com</t>
+  </si>
+  <si>
+    <t>MCA</t>
+  </si>
+  <si>
+    <t>BCA</t>
+  </si>
+  <si>
+    <t>BTECH</t>
+  </si>
+  <si>
+    <t>BE</t>
+  </si>
+  <si>
+    <t>MBA</t>
+  </si>
+  <si>
+    <t>CS</t>
+  </si>
+  <si>
+    <t>BCOM</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -52,13 +123,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -358,23 +432,155 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N18" sqref="N18"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14" customWidth="1"/>
+    <col min="2" max="2" width="15" customWidth="1"/>
+    <col min="3" max="3" width="30.28515625" customWidth="1"/>
+    <col min="4" max="4" width="13.28515625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9" t="s">
+        <v>18</v>
+      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1"/>
+    <hyperlink ref="B3" r:id="rId2"/>
+    <hyperlink ref="B4:B9" r:id="rId3" display="Test@123"/>
+    <hyperlink ref="C2" r:id="rId4"/>
+    <hyperlink ref="C3" r:id="rId5"/>
+    <hyperlink ref="C4:C9" r:id="rId6" display="user@user.com"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>